<commit_message>
Added Credit FCG Test Data and updated CrdeitThem script.
</commit_message>
<xml_diff>
--- a/KatalonData/VoidCreditThem.xlsx
+++ b/KatalonData/VoidCreditThem.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F088B5E-C470-45D6-8F3C-1E616170AAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB286DCE-F232-43F1-979B-F1C81F365AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="1545" windowWidth="24525" windowHeight="14010" xr2:uid="{68A01D60-C0DA-4B1C-A077-755B50774099}"/>
+    <workbookView xWindow="-26500" yWindow="3760" windowWidth="23040" windowHeight="12200" activeTab="1" xr2:uid="{68A01D60-C0DA-4B1C-A077-755B50774099}"/>
   </bookViews>
   <sheets>
     <sheet name="CreditThem" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
-    <sheet name="VoidThem" sheetId="2" r:id="rId4"/>
+    <sheet name="CreditFCG" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="VoidThem" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CreditThem!$A$1:$A$282</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">VoidThem!$A$1:$A$272</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">VoidThem!$A$1:$A$272</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="623">
   <si>
     <t>TransactionID</t>
   </si>
@@ -1720,6 +1721,198 @@
   </si>
   <si>
     <t>Thu Jan 18 19:32:23 EST 2024</t>
+  </si>
+  <si>
+    <t>322991949</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:29:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:41:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:41:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:42:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:42:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:42:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:43:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:43:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:43:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:45:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:45:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:46:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:46:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:46:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:47:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:47:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:47:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:48:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:48:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:48:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:49:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:49:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:49:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:50:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:50:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:50:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:51:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:51:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:51:51 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:52:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:52:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:52:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:53:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:53:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:53:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:54:11 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:54:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:54:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:55:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:55:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:55:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:56:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:56:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:56:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:57:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:57:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:57:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:58:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:58:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:58:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:59:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:59:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 17:59:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:00:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:00:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:00:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:01:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:01:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:01:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:02:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue Jul 09 18:02:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>322991884</t>
+  </si>
+  <si>
+    <t>322991924</t>
   </si>
 </sst>
 </file>
@@ -1735,12 +1928,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1770,7 +1969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1782,6 +1981,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1800,9 +2002,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1840,7 +2042,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1946,7 +2148,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2088,7 +2290,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E532ABCF-DAB7-44D4-A3CE-3A31591BDD05}">
   <dimension ref="A1:F282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6040,6 +6242,713 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFDD0FF-9C7F-42B8-8C7C-70B03C87DED6}">
+  <dimension ref="A1:D62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection sqref="A1:D62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.85546875" style="6" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="D3" s="6">
+        <v>322991947</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="D4" s="6">
+        <v>322991937</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="D5" s="6">
+        <v>322991933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="D6" s="6">
+        <v>322991929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="D8" s="6">
+        <v>322991914</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="D9" s="6">
+        <v>322991910</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="D10" s="6">
+        <v>322991907</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="D11" s="6">
+        <v>322991902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="D12" s="6">
+        <v>322991900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="D13" s="6">
+        <v>322991895</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="D14" s="6">
+        <v>322991893</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="D16" s="6">
+        <v>322991875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="D17" s="6">
+        <v>322991874</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="D18" s="6">
+        <v>322991871</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="D19" s="6">
+        <v>322991859</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="D20" s="6">
+        <v>322991851</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="D21" s="6">
+        <v>322991846</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="D22" s="6">
+        <v>322991833</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="D23" s="6">
+        <v>322991830</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="D24" s="6">
+        <v>322991824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="D25" s="6">
+        <v>322991818</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="D26" s="6">
+        <v>322991813</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="D27" s="6">
+        <v>322991805</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="D28" s="6">
+        <v>322991802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="D29" s="6">
+        <v>322991794</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="D30" s="6">
+        <v>322991782</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="D31" s="6">
+        <v>322991775</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="D32" s="6">
+        <v>322991774</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="D33" s="6">
+        <v>322991772</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="D34" s="6">
+        <v>322991765</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="D35" s="6">
+        <v>322991760</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="D36" s="6">
+        <v>322991758</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="D37" s="6">
+        <v>322991755</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="D38" s="6">
+        <v>322991744</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="D39" s="6">
+        <v>322991743</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="D40" s="6">
+        <v>322991740</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="D41" s="6">
+        <v>322991728</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="D42" s="6">
+        <v>322991727</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="D43" s="6">
+        <v>322991726</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="D44" s="6">
+        <v>322991721</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="D45" s="6">
+        <v>322991711</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="D46" s="6">
+        <v>322991710</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D47" s="6">
+        <v>322991700</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="D48" s="6">
+        <v>322991681</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="D49" s="6">
+        <v>322991651</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="D50" s="6">
+        <v>322991646</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="D51" s="6">
+        <v>322991622</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="D52" s="6">
+        <v>322991611</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="D53" s="6">
+        <v>322991605</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="D54" s="6">
+        <v>322991603</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="D55" s="6">
+        <v>322991598</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="D56" s="6">
+        <v>322991585</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="D57" s="6">
+        <v>322991563</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="D58" s="6">
+        <v>322991561</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="D59" s="6">
+        <v>322915933</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="D60" s="6">
+        <v>322915000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="D61" s="6">
+        <v>322898212</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="D62" s="6">
+        <v>322840887</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91561C24-D1D2-4B16-8C0B-8E7D28B8B97D}">
   <dimension ref="A1:D272"/>
   <sheetViews>
@@ -7429,7 +8338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34221211-C528-4B9A-8EB9-3F2A8222C832}">
   <dimension ref="A1:A8"/>
   <sheetViews>
@@ -7487,7 +8396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72837C1-A250-4429-940A-47740C3A20D1}">
   <dimension ref="A1:F272"/>
   <sheetViews>
@@ -11316,6 +12225,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="acacf6df-7f2b-4e22-b0f3-7512e3e41353" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4BE33D85B624C499A4F208BDFBE25E3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cd1df8248d0147635b68617ab35c068">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a46146ca-227b-4078-8d7d-54f809a0c7c3" xmlns:ns4="acacf6df-7f2b-4e22-b0f3-7512e3e41353" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="644d45e4cbba221d591cefd09b775554" ns3:_="" ns4:_="">
     <xsd:import namespace="a46146ca-227b-4078-8d7d-54f809a0c7c3"/>
@@ -11540,7 +12457,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11549,15 +12466,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="acacf6df-7f2b-4e22-b0f3-7512e3e41353" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F3410C-C74A-41CF-8658-138963324197}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="acacf6df-7f2b-4e22-b0f3-7512e3e41353"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a46146ca-227b-4078-8d7d-54f809a0c7c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9EA28B5-2EA2-4B32-A392-7713D681EE24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11576,27 +12502,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92B33282-DA3D-42FE-BA2A-24C428B7C579}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35F3410C-C74A-41CF-8658-138963324197}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="acacf6df-7f2b-4e22-b0f3-7512e3e41353"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a46146ca-227b-4078-8d7d-54f809a0c7c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>